<commit_message>
Updated the example for reading a deviant file. Set extra option for page width. Added some page layout.
</commit_message>
<xml_diff>
--- a/pkg/vignettes/test.xlsx
+++ b/pkg/vignettes/test.xlsx
@@ -42,12 +42,6 @@
     <t>Inkh</t>
   </si>
   <si>
-    <t>Willekeurige afschrijving investeringen in 2009</t>
-  </si>
-  <si>
-    <t>vervallen vrijstelling MRB auto's &gt; 25 jr</t>
-  </si>
-  <si>
     <t>Mb</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>kt</t>
+  </si>
+  <si>
+    <t>Willekeurige afschrijving investeringen</t>
+  </si>
+  <si>
+    <t>Vervallen vrijstelling MRB auto's&gt;25jr</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +428,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>